<commit_message>
Added pseudo code that i have doe as of today please check and reply asap with comments
</commit_message>
<xml_diff>
--- a/Pseudo Code/playerClass.xlsx
+++ b/Pseudo Code/playerClass.xlsx
@@ -155,9 +155,6 @@
     <t xml:space="preserve">\\ got full training value so looses more health than usual </t>
   </si>
   <si>
-    <t>public boolean getInjured(health int)</t>
-  </si>
-  <si>
     <t>getInjured(health int)</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>end getInjured</t>
+  </si>
+  <si>
+    <t>public boolean getInjured(health int, player id)</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>41</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -741,17 +741,17 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
@@ -804,12 +804,12 @@
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
@@ -819,12 +819,12 @@
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
@@ -834,12 +834,12 @@
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
@@ -849,12 +849,12 @@
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>